<commit_message>
Commit on 2025-02-21 07:42:35
</commit_message>
<xml_diff>
--- a/H02_海外債券交易/01_基礎應用/EXE/price_information.xlsx
+++ b/H02_海外債券交易/01_基礎應用/EXE/price_information.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,102 +436,107 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>證券編碼</t>
+          <t>isin</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>最新價格</t>
+          <t>lastPrice</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>最新價格時間戳</t>
+          <t>timestampLastPrice</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>今日漲跌價格</t>
+          <t>changeToPrevDayAbsolute</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>今日漲跌幅度</t>
+          <t>changeToPrevDayInPercent</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>前日收盤價</t>
+          <t>closingPricePrevTradingDay</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>市場識別碼</t>
+          <t>mic</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>最高價</t>
+          <t>lastPriceIndicator</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>最低價</t>
+          <t>dayHigh</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>價格定點</t>
+          <t>dayLow</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>以百分比交易</t>
+          <t>priceFixings</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>交易結束時間</t>
+          <t>tradedInPercent</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>交易開始時間</t>
+          <t>tradingTimeEnd</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>成交額（歐元）</t>
+          <t>tradingTimeStart</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>成交量（件數）</t>
+          <t>turnoverInEur</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>名義成交額</t>
+          <t>turnoverInPieces</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>52週最高價</t>
+          <t>turnoverNominal</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>52週最低價</t>
+          <t>weeks52High</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>貨幣</t>
+          <t>weeks52Low</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>最小可交易單位</t>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>minimumTradableUnit</t>
         </is>
       </c>
     </row>
@@ -542,66 +547,69 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>97.17</v>
+        <v>90.44</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2023-12-14 16:44</t>
+          <t>2025-02-20T10:18:03+01:00</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2.7</v>
+        <v>0.37</v>
       </c>
       <c r="E2" t="n">
-        <v>2.8580501746</v>
+        <v>0.41</v>
       </c>
       <c r="F2" t="n">
-        <v>94.47</v>
+        <v>90.44</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>XFRA</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>97.17</v>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>97.17</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="b">
+        <v>90.44</v>
+      </c>
+      <c r="J2" t="n">
+        <v>90.44</v>
+      </c>
+      <c r="K2" t="n">
         <v>1</v>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2023-12-16 00:30</t>
-        </is>
+      <c r="L2" t="b">
+        <v>1</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2023-12-15 15:00</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
+          <t>17:30:00</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="n">
-        <v>101.39</v>
-      </c>
       <c r="R2" t="n">
-        <v>80.95</v>
-      </c>
-      <c r="S2" t="inlineStr">
+        <v>101.29</v>
+      </c>
+      <c r="S2" t="n">
+        <v>87.34</v>
+      </c>
+      <c r="T2" t="inlineStr">
         <is>
           <t>{'originalValue': 'USD', 'translations': {'de': 'US-Dollar', 'en': 'U.S. dollar'}}</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>200000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit on 2025-02-22 09:13:54
</commit_message>
<xml_diff>
--- a/H02_海外債券交易/01_基礎應用/EXE/price_information.xlsx
+++ b/H02_海外債券交易/01_基礎應用/EXE/price_information.xlsx
@@ -436,37 +436,37 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>isin</t>
+          <t>證券編碼</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>lastPrice</t>
+          <t>最新價格</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>timestampLastPrice</t>
+          <t>最新價格時間戳</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>changeToPrevDayAbsolute</t>
+          <t>今日漲跌價格</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>changeToPrevDayInPercent</t>
+          <t>今日漲跌幅度</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>closingPricePrevTradingDay</t>
+          <t>前日收盤價</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>mic</t>
+          <t>市場識別碼</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -476,67 +476,67 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>dayHigh</t>
+          <t>最高價</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>dayLow</t>
+          <t>最低價</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>priceFixings</t>
+          <t>價格定點</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>tradedInPercent</t>
+          <t>以百分比交易</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>tradingTimeEnd</t>
+          <t>交易結束時間</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>tradingTimeStart</t>
+          <t>交易開始時間</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>turnoverInEur</t>
+          <t>成交額（歐元）</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>turnoverInPieces</t>
+          <t>成交量（件數）</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>turnoverNominal</t>
+          <t>名義成交額</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>weeks52High</t>
+          <t>52週最高價</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>weeks52Low</t>
+          <t>52週最低價</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>貨幣</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>minimumTradableUnit</t>
+          <t>最小可交易單位</t>
         </is>
       </c>
     </row>
@@ -547,18 +547,18 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90.44</v>
+        <v>91</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-20T10:18:03+01:00</t>
+          <t>2025-02-21 16:37</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.37</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>0.41</v>
+        <v>0.62</v>
       </c>
       <c r="F2" t="n">
         <v>90.44</v>
@@ -570,10 +570,10 @@
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
-        <v>90.44</v>
+        <v>91</v>
       </c>
       <c r="J2" t="n">
-        <v>90.44</v>
+        <v>91</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>

</xml_diff>